<commit_message>
Added some comments for candidate-JSON
</commit_message>
<xml_diff>
--- a/codebook/codebook_elections2023.xlsx
+++ b/codebook/codebook_elections2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\wd-poku\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D006D-AE67-4099-8551-EA0BE5877483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8A1726-568A-4977-8E9B-1C6DF24DDC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{33CDBF25-DF6C-428D-82EC-BC4FA608AEC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{33CDBF25-DF6C-428D-82EC-BC4FA608AEC1}"/>
   </bookViews>
   <sheets>
     <sheet name="wahlbeteiligung" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="250">
   <si>
     <t>Node</t>
   </si>
@@ -752,9 +752,6 @@
     <t>Date of birth of candidate</t>
   </si>
   <si>
-    <t>For candidates living abroad, 9950 is assigned as municipality number</t>
-  </si>
-  <si>
     <t>FSO list number (numeric))</t>
   </si>
   <si>
@@ -779,32 +776,26 @@
     <t>Only for cantons with proportional representation system.; The party LPS/PLS (FSO party number=5) was assigned to that of FDP/PLR (FSO party number=1) for level_ch for all data years.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">null: candidate has never been elected before; 2: incumbent; </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>3: former (candidate has already been elected in the past)</t>
-    </r>
-  </si>
-  <si>
     <t>see metadaten.json; The value =3 (ehemalig/ancien/ne élu/e/già eletto/a in passato/former) can no longer be supplied for 2023. The structure of the variable is retained.</t>
   </si>
   <si>
     <t>Update 20230821: not considered as critical variable. Will be supplied normally.</t>
+  </si>
+  <si>
+    <t>2= incumbent; else value='null'</t>
+  </si>
+  <si>
+    <t>Indication by candidate when registering candidacy.</t>
+  </si>
+  <si>
+    <t>The number (ID) is only supplied after the periods allowed for rectifications in all cantons have expired. The municipality number is added on the basis of address data by the FSO. For candidates living abroad, 9950 is assigned as municipality number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,13 +817,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1178,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6385737F-2AEE-469B-86AC-899DE5827E87}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -1293,7 +1277,7 @@
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1361,7 +1345,7 @@
         <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1589,7 +1573,7 @@
         <v>108</v>
       </c>
       <c r="E37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1712,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E575B35C-1FAB-45CB-BCF6-DB597EE2D0F3}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1870,7 +1854,7 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2049,7 +2033,7 @@
         <v>96</v>
       </c>
       <c r="E30" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
@@ -2062,6 +2046,9 @@
       <c r="D31" t="s">
         <v>98</v>
       </c>
+      <c r="E31" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
@@ -2085,10 +2072,10 @@
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E33" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2135,7 +2122,7 @@
         <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2160,7 +2147,7 @@
         <v>108</v>
       </c>
       <c r="E39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2182,7 +2169,7 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2387,7 +2374,7 @@
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2455,7 +2442,7 @@
         <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -2539,7 +2526,7 @@
         <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -2553,7 +2540,7 @@
         <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -2567,7 +2554,7 @@
         <v>125</v>
       </c>
       <c r="E24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
@@ -2765,7 +2752,7 @@
         <v>103</v>
       </c>
       <c r="E42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2835,7 +2822,7 @@
         <v>158</v>
       </c>
       <c r="E47" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2849,7 +2836,7 @@
         <v>159</v>
       </c>
       <c r="E48" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
@@ -2863,7 +2850,7 @@
         <v>160</v>
       </c>
       <c r="E49" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
@@ -3072,7 +3059,7 @@
         <v>108</v>
       </c>
       <c r="E68" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -3373,7 +3360,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3451,7 +3438,7 @@
         <v>194</v>
       </c>
       <c r="E21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -3676,7 +3663,7 @@
         <v>206</v>
       </c>
       <c r="E16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3690,7 +3677,7 @@
         <v>207</v>
       </c>
       <c r="E17" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3704,7 +3691,7 @@
         <v>208</v>
       </c>
       <c r="E18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3834,7 +3821,7 @@
         <v>215</v>
       </c>
       <c r="E29" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3848,7 +3835,7 @@
         <v>216</v>
       </c>
       <c r="E30" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -3862,7 +3849,7 @@
         <v>217</v>
       </c>
       <c r="E31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -4002,7 +3989,7 @@
         <v>202</v>
       </c>
       <c r="E11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -4016,7 +4003,7 @@
         <v>203</v>
       </c>
       <c r="E12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -4030,7 +4017,7 @@
         <v>204</v>
       </c>
       <c r="E13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -4044,7 +4031,7 @@
         <v>205</v>
       </c>
       <c r="E14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4069,7 +4056,7 @@
         <v>206</v>
       </c>
       <c r="E16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -4083,7 +4070,7 @@
         <v>207</v>
       </c>
       <c r="E17" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -4097,7 +4084,7 @@
         <v>208</v>
       </c>
       <c r="E18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -4252,7 +4239,7 @@
         <v>215</v>
       </c>
       <c r="E31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -4266,7 +4253,7 @@
         <v>216</v>
       </c>
       <c r="E32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
@@ -4280,7 +4267,7 @@
         <v>217</v>
       </c>
       <c r="E33" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed Intro-text and added testing-information
</commit_message>
<xml_diff>
--- a/codebook/codebook_elections2023.xlsx
+++ b/codebook/codebook_elections2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\wd-poku\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8A1726-568A-4977-8E9B-1C6DF24DDC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20125705-7398-40A2-BBFE-72267E8CA7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{33CDBF25-DF6C-428D-82EC-BC4FA608AEC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{33CDBF25-DF6C-428D-82EC-BC4FA608AEC1}"/>
   </bookViews>
   <sheets>
     <sheet name="wahlbeteiligung" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="251">
   <si>
     <t>Node</t>
   </si>
@@ -789,6 +789,9 @@
   </si>
   <si>
     <t>The number (ID) is only supplied after the periods allowed for rectifications in all cantons have expired. The municipality number is added on the basis of address data by the FSO. For candidates living abroad, 9950 is assigned as municipality number</t>
+  </si>
+  <si>
+    <t>level_ch: Will be filled as soon as the election is completed</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E575B35C-1FAB-45CB-BCF6-DB597EE2D0F3}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -2266,7 +2269,7 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3197,7 +3200,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3473,7 +3476,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3562,6 +3565,9 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
+      <c r="E8" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -3697,6 +3703,9 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3862,8 +3871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D99236-7A0F-4410-A26F-58A0A36CFCB4}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3952,6 +3961,9 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
+      <c r="E8" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -4112,6 +4124,9 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
infos on CS and update info page
</commit_message>
<xml_diff>
--- a/codebook/codebook_elections2023.xlsx
+++ b/codebook/codebook_elections2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\wd-poku\codebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\wd-poku.new\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A486F70-6EB5-4A9B-973A-15A7A807966C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47416843-3036-4C4A-A3F0-DD812241DAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="6" xr2:uid="{33CDBF25-DF6C-428D-82EC-BC4FA608AEC1}"/>
+    <workbookView xWindow="-13944" yWindow="-16308" windowWidth="29016" windowHeight="15816" activeTab="2" xr2:uid="{33CDBF25-DF6C-428D-82EC-BC4FA608AEC1}"/>
   </bookViews>
   <sheets>
     <sheet name="wahlbeteiligung" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="zeitreihen-frauen-beteiligung" sheetId="6" r:id="rId5"/>
     <sheet name="zeitreihen-parteien" sheetId="7" r:id="rId6"/>
     <sheet name="listen-gde" sheetId="8" r:id="rId7"/>
+    <sheet name="SRW" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="276">
   <si>
     <t>Node</t>
   </si>
@@ -799,6 +800,75 @@
   </si>
   <si>
     <t>Number of total votes per list; level: municipality</t>
+  </si>
+  <si>
+    <t>wahlgang</t>
+  </si>
+  <si>
+    <t>Round of voting</t>
+  </si>
+  <si>
+    <t>wahlgang_abgeschlossen</t>
+  </si>
+  <si>
+    <t>Indicates that all cantons have delivered their provisional final result for a given round of voting (boolean true/false)</t>
+  </si>
+  <si>
+    <t>Number of cantons that have delivered their provisional final result for a given round of voting</t>
+  </si>
+  <si>
+    <t>wahlgang_datum</t>
+  </si>
+  <si>
+    <t>Date of the election round</t>
+  </si>
+  <si>
+    <t>stille_wahl</t>
+  </si>
+  <si>
+    <t>True if tacit election. Electoral procedure in which the cantonal government declares the person(s) as elected because there were no more candidates than mandates to be allocated.</t>
+  </si>
+  <si>
+    <t>zweiter_wahlgang_noetig</t>
+  </si>
+  <si>
+    <t>Indicates whether a second round of voting is necessary in a given canton</t>
+  </si>
+  <si>
+    <t>Indicates whether the respective round of voting is completed in a given canton</t>
+  </si>
+  <si>
+    <t>kandidierende</t>
+  </si>
+  <si>
+    <t>Update interval per completed canton</t>
+  </si>
+  <si>
+    <t>date string</t>
+  </si>
+  <si>
+    <t>see metadaten.json; The value =3 (ehemalig/ancien/ne élu/e/già eletto/a in passato/former) can no longer be supplied for 2023.</t>
+  </si>
+  <si>
+    <t>Number of votes candidate has received</t>
+  </si>
+  <si>
+    <t>Only for first round of voting (if wahlgang = 1)</t>
+  </si>
+  <si>
+    <t>For the second round, the flag is set once the cantons has declared the validity of the single candidature.</t>
+  </si>
+  <si>
+    <t>For election rounds with tacit election (stille_wahl = 1), the original intended date of the election is given.</t>
+  </si>
+  <si>
+    <t>In case of a tacit election, the flag is set once the canton has declared the candidate as elected.</t>
+  </si>
+  <si>
+    <t>will be null in case of tacit election</t>
+  </si>
+  <si>
+    <t>In 2021 the CVP (partei_id = 2) merged with the BDP (partei_id = 34) under the name "Die Mitte" / "Centre". For the direct comparison of the election years 2023 and 2019, the party results of CVP and BDP  are combined for 2019 and shown as results for the Centre party (partei_id = 34).</t>
   </si>
 </sst>
 </file>
@@ -1172,19 +1242,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6385737F-2AEE-469B-86AC-899DE5827E87}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="97.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1271,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1212,7 +1282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1237,13 +1307,13 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1254,7 +1324,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1265,7 +1335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -1276,7 +1346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -1290,7 +1360,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1301,12 +1371,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -1317,7 +1387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -1328,7 +1398,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -1339,7 +1409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1350,7 +1420,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1358,7 +1428,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -1369,7 +1439,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>35</v>
       </c>
@@ -1380,7 +1450,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>37</v>
       </c>
@@ -1391,7 +1461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>39</v>
       </c>
@@ -1402,7 +1472,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>41</v>
       </c>
@@ -1413,7 +1483,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>43</v>
       </c>
@@ -1424,7 +1494,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>46</v>
       </c>
@@ -1435,7 +1505,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>48</v>
       </c>
@@ -1446,7 +1516,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1454,7 +1524,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>26</v>
       </c>
@@ -1465,7 +1535,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>51</v>
       </c>
@@ -1476,7 +1546,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>33</v>
       </c>
@@ -1487,7 +1557,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -1498,7 +1568,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>37</v>
       </c>
@@ -1509,7 +1579,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -1520,7 +1590,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>41</v>
       </c>
@@ -1531,7 +1601,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>43</v>
       </c>
@@ -1542,7 +1612,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>46</v>
       </c>
@@ -1553,7 +1623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>48</v>
       </c>
@@ -1564,7 +1634,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>62</v>
       </c>
@@ -1572,7 +1642,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>63</v>
       </c>
@@ -1586,7 +1656,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>64</v>
       </c>
@@ -1597,7 +1667,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>26</v>
       </c>
@@ -1608,7 +1678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>33</v>
       </c>
@@ -1619,7 +1689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>35</v>
       </c>
@@ -1630,7 +1700,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>37</v>
       </c>
@@ -1641,7 +1711,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>39</v>
       </c>
@@ -1652,7 +1722,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>41</v>
       </c>
@@ -1663,7 +1733,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -1674,7 +1744,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>46</v>
       </c>
@@ -1685,7 +1755,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>48</v>
       </c>
@@ -1706,19 +1776,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E575B35C-1FAB-45CB-BCF6-DB597EE2D0F3}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1805,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1743,7 +1813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1754,7 +1824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1765,13 +1835,13 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1782,7 +1852,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1793,7 +1863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -1804,7 +1874,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -1815,7 +1885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1826,12 +1896,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -1842,7 +1912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -1853,7 +1923,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -1867,7 +1937,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1878,7 +1948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1886,7 +1956,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>26</v>
       </c>
@@ -1897,7 +1967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>51</v>
       </c>
@@ -1908,7 +1978,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>75</v>
       </c>
@@ -1919,7 +1989,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>76</v>
       </c>
@@ -1930,7 +2000,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>77</v>
       </c>
@@ -1941,7 +2011,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>79</v>
       </c>
@@ -1952,7 +2022,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>81</v>
       </c>
@@ -1963,7 +2033,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>83</v>
       </c>
@@ -1974,7 +2044,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>85</v>
       </c>
@@ -1985,7 +2055,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>87</v>
       </c>
@@ -1996,7 +2066,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>89</v>
       </c>
@@ -2010,7 +2080,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>91</v>
       </c>
@@ -2021,7 +2091,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>93</v>
       </c>
@@ -2032,7 +2102,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>95</v>
       </c>
@@ -2046,7 +2116,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>97</v>
       </c>
@@ -2060,7 +2130,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>99</v>
       </c>
@@ -2074,7 +2144,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>101</v>
       </c>
@@ -2088,7 +2158,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>102</v>
       </c>
@@ -2102,7 +2172,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>104</v>
       </c>
@@ -2113,7 +2183,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>106</v>
       </c>
@@ -2127,7 +2197,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -2135,7 +2205,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>26</v>
       </c>
@@ -2146,7 +2216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>63</v>
       </c>
@@ -2160,7 +2230,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>64</v>
       </c>
@@ -2171,7 +2241,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>75</v>
       </c>
@@ -2182,7 +2252,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>76</v>
       </c>
@@ -2193,7 +2263,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>79</v>
       </c>
@@ -2204,7 +2274,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>85</v>
       </c>
@@ -2215,7 +2285,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>87</v>
       </c>
@@ -2226,7 +2296,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>102</v>
       </c>
@@ -2240,7 +2310,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>104</v>
       </c>
@@ -2251,7 +2321,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>106</v>
       </c>
@@ -2275,19 +2345,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC8C16E-0A7E-4DE3-9CE5-9AF5B2628BEF}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E69"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="101.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2304,7 +2372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2312,7 +2380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2323,7 +2391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2334,13 +2402,13 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -2351,7 +2419,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -2362,7 +2430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -2373,7 +2441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -2387,7 +2455,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -2398,7 +2466,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>26</v>
       </c>
@@ -2409,12 +2477,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -2425,7 +2493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -2436,7 +2504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -2447,7 +2515,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2455,7 +2523,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>111</v>
       </c>
@@ -2469,7 +2537,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>112</v>
       </c>
@@ -2483,7 +2551,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>114</v>
       </c>
@@ -2497,7 +2565,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>116</v>
       </c>
@@ -2511,7 +2579,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>118</v>
       </c>
@@ -2525,7 +2593,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>120</v>
       </c>
@@ -2539,7 +2607,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>122</v>
       </c>
@@ -2553,7 +2621,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>124</v>
       </c>
@@ -2567,7 +2635,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>126</v>
       </c>
@@ -2577,8 +2645,11 @@
       <c r="D25" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>128</v>
       </c>
@@ -2588,8 +2659,11 @@
       <c r="D26" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>130</v>
       </c>
@@ -2599,8 +2673,11 @@
       <c r="D27" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>132</v>
       </c>
@@ -2610,8 +2687,11 @@
       <c r="D28" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>134</v>
       </c>
@@ -2621,8 +2701,11 @@
       <c r="D29" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>136</v>
       </c>
@@ -2632,8 +2715,11 @@
       <c r="D30" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>138</v>
       </c>
@@ -2644,7 +2730,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>140</v>
       </c>
@@ -2654,8 +2740,11 @@
       <c r="D32" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>142</v>
       </c>
@@ -2665,8 +2754,11 @@
       <c r="D33" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>144</v>
       </c>
@@ -2677,7 +2769,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>146</v>
       </c>
@@ -2687,8 +2779,11 @@
       <c r="D35" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>148</v>
       </c>
@@ -2698,8 +2793,11 @@
       <c r="D36" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>150</v>
       </c>
@@ -2710,7 +2808,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>152</v>
       </c>
@@ -2721,7 +2819,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2729,7 +2827,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>26</v>
       </c>
@@ -2740,7 +2838,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>51</v>
       </c>
@@ -2751,7 +2849,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>111</v>
       </c>
@@ -2765,7 +2863,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>112</v>
       </c>
@@ -2779,7 +2877,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>114</v>
       </c>
@@ -2793,7 +2891,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>116</v>
       </c>
@@ -2807,7 +2905,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>118</v>
       </c>
@@ -2821,7 +2919,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>120</v>
       </c>
@@ -2835,7 +2933,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>122</v>
       </c>
@@ -2849,7 +2947,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>124</v>
       </c>
@@ -2863,7 +2961,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>126</v>
       </c>
@@ -2873,8 +2971,11 @@
       <c r="D50" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>128</v>
       </c>
@@ -2884,8 +2985,11 @@
       <c r="D51" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>130</v>
       </c>
@@ -2895,8 +2999,11 @@
       <c r="D52" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>132</v>
       </c>
@@ -2906,8 +3013,11 @@
       <c r="D53" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>134</v>
       </c>
@@ -2917,8 +3027,11 @@
       <c r="D54" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>136</v>
       </c>
@@ -2928,8 +3041,11 @@
       <c r="D55" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>138</v>
       </c>
@@ -2940,7 +3056,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>140</v>
       </c>
@@ -2950,8 +3066,11 @@
       <c r="D57" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>142</v>
       </c>
@@ -2961,8 +3080,11 @@
       <c r="D58" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>170</v>
       </c>
@@ -2973,7 +3095,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>172</v>
       </c>
@@ -2983,8 +3105,11 @@
       <c r="D60" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>174</v>
       </c>
@@ -2994,8 +3119,11 @@
       <c r="D61" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>144</v>
       </c>
@@ -3006,7 +3134,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>146</v>
       </c>
@@ -3016,8 +3144,11 @@
       <c r="D63" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>148</v>
       </c>
@@ -3027,8 +3158,11 @@
       <c r="D64" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>150</v>
       </c>
@@ -3039,7 +3173,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>152</v>
       </c>
@@ -3050,7 +3184,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -3058,7 +3192,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>63</v>
       </c>
@@ -3072,7 +3206,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>64</v>
       </c>
@@ -3083,7 +3217,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>26</v>
       </c>
@@ -3094,7 +3228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>111</v>
       </c>
@@ -3108,7 +3242,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>170</v>
       </c>
@@ -3119,7 +3253,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>172</v>
       </c>
@@ -3129,8 +3263,11 @@
       <c r="D73" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>174</v>
       </c>
@@ -3140,8 +3277,11 @@
       <c r="D74" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>144</v>
       </c>
@@ -3152,7 +3292,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>146</v>
       </c>
@@ -3162,8 +3302,11 @@
       <c r="D76" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>148</v>
       </c>
@@ -3173,8 +3316,11 @@
       <c r="D77" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>150</v>
       </c>
@@ -3185,7 +3331,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>152</v>
       </c>
@@ -3210,14 +3356,14 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="85.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3234,7 +3380,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3242,7 +3388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3253,7 +3399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3265,14 +3411,14 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -3283,7 +3429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -3294,7 +3440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -3305,12 +3451,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -3321,7 +3467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -3332,7 +3478,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3340,7 +3486,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -3351,7 +3497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>51</v>
       </c>
@@ -3362,7 +3508,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>75</v>
       </c>
@@ -3373,7 +3519,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>76</v>
       </c>
@@ -3384,7 +3530,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>77</v>
       </c>
@@ -3395,7 +3541,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>190</v>
       </c>
@@ -3409,7 +3555,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>192</v>
       </c>
@@ -3423,7 +3569,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>111</v>
       </c>
@@ -3437,7 +3583,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>120</v>
       </c>
@@ -3451,7 +3597,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>195</v>
       </c>
@@ -3462,7 +3608,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>197</v>
       </c>
@@ -3486,15 +3632,15 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3511,7 +3657,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3519,7 +3665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3530,12 +3676,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3546,7 +3692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -3557,7 +3703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -3568,7 +3714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3576,7 +3722,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -3587,7 +3733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -3598,7 +3744,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>201</v>
       </c>
@@ -3609,7 +3755,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>112</v>
       </c>
@@ -3623,7 +3769,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>114</v>
       </c>
@@ -3637,7 +3783,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>116</v>
       </c>
@@ -3651,7 +3797,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>118</v>
       </c>
@@ -3665,7 +3811,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>120</v>
       </c>
@@ -3679,7 +3825,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>122</v>
       </c>
@@ -3693,7 +3839,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>124</v>
       </c>
@@ -3707,7 +3853,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -3715,7 +3861,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>26</v>
       </c>
@@ -3726,7 +3872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>209</v>
       </c>
@@ -3737,7 +3883,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -3748,7 +3894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>43</v>
       </c>
@@ -3759,7 +3905,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>201</v>
       </c>
@@ -3770,7 +3916,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>112</v>
       </c>
@@ -3784,7 +3930,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>114</v>
       </c>
@@ -3798,7 +3944,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>116</v>
       </c>
@@ -3812,7 +3958,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>118</v>
       </c>
@@ -3826,7 +3972,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>120</v>
       </c>
@@ -3840,7 +3986,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>122</v>
       </c>
@@ -3854,7 +4000,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>124</v>
       </c>
@@ -3882,15 +4028,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3907,7 +4053,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3915,7 +4061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3926,12 +4072,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3942,7 +4088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -3953,7 +4099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -3964,7 +4110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3972,7 +4118,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -3983,7 +4129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>111</v>
       </c>
@@ -3997,7 +4143,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>112</v>
       </c>
@@ -4011,7 +4157,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>114</v>
       </c>
@@ -4025,7 +4171,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>116</v>
       </c>
@@ -4039,7 +4185,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>118</v>
       </c>
@@ -4053,7 +4199,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>144</v>
       </c>
@@ -4064,7 +4210,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>120</v>
       </c>
@@ -4078,7 +4224,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>122</v>
       </c>
@@ -4092,7 +4238,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>124</v>
       </c>
@@ -4106,7 +4252,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>201</v>
       </c>
@@ -4117,7 +4263,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>152</v>
       </c>
@@ -4128,7 +4274,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -4136,7 +4282,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -4147,7 +4293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>51</v>
       </c>
@@ -4158,7 +4304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -4169,7 +4315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>111</v>
       </c>
@@ -4183,7 +4329,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>112</v>
       </c>
@@ -4197,7 +4343,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>114</v>
       </c>
@@ -4211,7 +4357,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>116</v>
       </c>
@@ -4225,7 +4371,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>118</v>
       </c>
@@ -4239,7 +4385,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>144</v>
       </c>
@@ -4250,7 +4396,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>120</v>
       </c>
@@ -4264,7 +4410,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>122</v>
       </c>
@@ -4278,7 +4424,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>124</v>
       </c>
@@ -4292,7 +4438,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>201</v>
       </c>
@@ -4303,7 +4449,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>152</v>
       </c>
@@ -4323,18 +4469,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBEAE3D-B5A1-46F3-A39F-183AD43B2E3E}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="85.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4351,7 +4497,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4359,7 +4505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -4367,7 +4513,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>26</v>
       </c>
@@ -4378,7 +4524,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>51</v>
       </c>
@@ -4389,7 +4535,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -4403,7 +4549,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -4414,7 +4560,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -4425,7 +4571,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>76</v>
       </c>
@@ -4436,7 +4582,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>111</v>
       </c>
@@ -4450,7 +4596,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>195</v>
       </c>
@@ -4459,6 +4605,330 @@
       </c>
       <c r="D11" t="s">
         <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56C7-CA89-4283-BA7D-3A602D820FA0}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>265</v>
+      </c>
+      <c r="E15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>247</v>
+      </c>
+      <c r="E23" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>269</v>
+      </c>
+      <c r="E26" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>